<commit_message>
fix: Tableau CARIF avec lieu de formation
</commit_message>
<xml_diff>
--- a/public/modeles/export_carif.xlsx
+++ b/public/modeles/export_carif.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA7F458-F6CF-F64D-B79E-B80F69C4A5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BE69B9-555D-D540-A68C-5D8F8320BBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{C32C33F6-18C2-C24B-97D0-9EC3ED21FBB6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Composante</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Validation CFVU</t>
+  </si>
+  <si>
+    <t>Site formation</t>
   </si>
 </sst>
 </file>
@@ -98,9 +101,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,48 +417,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED77676A-A835-B84D-A6BB-EAF0C65610B1}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>